<commit_message>
Alteração do responsável para JOSÉ nos mapas IQ*
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IQ_CQ.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IQ_CQ.XLSX
@@ -334,10 +334,10 @@
 CQ</t>
   </si>
   <si>
-    <t>RODOLFO LUIZ DE MATOS</t>
-  </si>
-  <si>
-    <t>Matr.: 3416</t>
+    <t>JOSÉ DE CASTRO DA SILVA JUNIOR</t>
+  </si>
+  <si>
+    <t>Matr.: 3345</t>
   </si>
   <si>
     <t>IQ_CQ</t>

</xml_diff>